<commit_message>
working on buy manager
</commit_message>
<xml_diff>
--- a/application/plugins/StockBuyManager/views/StockBuyExport.xlsx
+++ b/application/plugins/StockBuyManager/views/StockBuyExport.xlsx
@@ -58,91 +58,91 @@
     <t>кг</t>
   </si>
   <si>
-    <t>Товары поставщиков</t>
-  </si>
-  <si>
-    <t>{$rows[]-&gt;supplier_name}</t>
-  </si>
-  <si>
-    <t>{$rows[]-&gt;supply_code}</t>
-  </si>
-  <si>
-    <t>{$rows[]-&gt;supply_name}</t>
-  </si>
-  <si>
-    <t>{$rows[]-&gt;supply_self}</t>
-  </si>
-  <si>
-    <t>{$rows[]-&gt;supply_buy}</t>
-  </si>
-  <si>
-    <t>{$rows[]-&gt;supply_sell}</t>
-  </si>
-  <si>
-    <t>{$rows[]-&gt;supply_comment}</t>
-  </si>
-  <si>
-    <t>{$rows[]-&gt;product_code}</t>
-  </si>
-  <si>
-    <t>{$rows[]-&gt;supply_modified}</t>
-  </si>
-  <si>
-    <t>{$rows[]-&gt;supply_spack}</t>
-  </si>
-  <si>
-    <t>{$rows[]-&gt;supply_bpack}</t>
-  </si>
-  <si>
-    <t>{$rows[]-&gt;supply_volume}</t>
-  </si>
-  <si>
-    <t>{$rows[]-&gt;supply_weight}</t>
-  </si>
-  <si>
-    <t>{$rows[]-&gt;supply_unit}</t>
-  </si>
-  <si>
-    <t>{$filter-&gt;supplier_name}</t>
-  </si>
-  <si>
-    <t>{$filter-&gt;supply_code}</t>
-  </si>
-  <si>
-    <t>{$filter-&gt;supply_name}</t>
-  </si>
-  <si>
-    <t>{$filter-&gt;supply_buy}</t>
-  </si>
-  <si>
-    <t>{$filter-&gt;supply_self}</t>
-  </si>
-  <si>
-    <t>{$filter-&gt;supply_sell}</t>
-  </si>
-  <si>
-    <t>{$filter-&gt;supply_comment}</t>
-  </si>
-  <si>
-    <t>{$filter-&gt;product_code}</t>
-  </si>
-  <si>
-    <t>{$filter-&gt;supply_modified}</t>
-  </si>
-  <si>
-    <t>{$filter-&gt;supply_spack}</t>
-  </si>
-  <si>
-    <t>{$filter-&gt;supply_bpack}</t>
-  </si>
-  <si>
-    <t>{$filter-&gt;supply_volume}</t>
-  </si>
-  <si>
-    <t>{$filter-&gt;supply_weight}</t>
-  </si>
-  <si>
-    <t>{$filter-&gt;supply_unit}</t>
+    <t>{$v-&gt;filter-&gt;supplier_name}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;filter-&gt;supply_code}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;filter-&gt;supply_name}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;filter-&gt;supply_buy}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;filter-&gt;supply_self}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;filter-&gt;supply_sell}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;filter-&gt;supply_comment}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;filter-&gt;product_code}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;filter-&gt;supply_modified}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;filter-&gt;supply_spack}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;filter-&gt;supply_bpack}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;filter-&gt;supply_volume}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;filter-&gt;supply_weight}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;filter-&gt;supply_unit}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;supplier_name}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;supply_code}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;supply_name}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;supply_buy}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;supply_self}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;supply_sell}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;supply_comment}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;product_code}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;supply_modified}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;supply_spack}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;supply_bpack}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;supply_volume}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;supply_weight}</t>
+  </si>
+  <si>
+    <t>{$v-&gt;rows[]-&gt;supply_unit}</t>
+  </si>
+  <si>
+    <t>Товары поставщиков {$v-&gt;date}</t>
   </si>
 </sst>
 </file>
@@ -191,7 +191,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -372,7 +372,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -380,8 +380,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -400,7 +399,24 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -705,7 +721,7 @@
   <dimension ref="A1:N5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="M4" sqref="L4:M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,153 +736,153 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="24" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="11"/>
+      <c r="A1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="10"/>
     </row>
-    <row r="2" spans="1:14" s="15" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="12" t="s">
+    <row r="2" spans="1:14" s="7" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="13" t="s">
+      <c r="F2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="G2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="H2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="13" t="s">
+      <c r="I2" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="13" t="s">
+      <c r="J2" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="13" t="s">
+      <c r="K2" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="13" t="s">
+      <c r="L2" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="13" t="s">
+      <c r="M2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="N2" s="13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>29</v>
+        <v>14</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>32</v>
+        <v>17</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>34</v>
+        <v>19</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>35</v>
+        <v>20</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="I3" s="5" t="s">
-        <v>37</v>
+        <v>22</v>
       </c>
       <c r="J3" s="5" t="s">
-        <v>38</v>
+        <v>23</v>
       </c>
       <c r="K3" s="5" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>41</v>
+        <v>26</v>
       </c>
       <c r="N3" s="6" t="s">
-        <v>42</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="L4" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="M4" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="N4" s="7" t="s">
+      <c r="A4" s="14" t="s">
         <v>28</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="J4" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="L4" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="M4" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="17" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>